<commit_message>
DNN 5000 results with 50000 unlabeled data obtained
</commit_message>
<xml_diff>
--- a/results/Lake/ComputationalTime.xlsx
+++ b/results/Lake/ComputationalTime.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20356"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939FDF20-F60A-4120-85C1-F854B6446E84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1511ED44-0A8F-4B7A-A99B-9566BC7CF174}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="6795" windowHeight="7290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t xml:space="preserve">DNN_loss_MC_p_Lake.py </t>
   </si>
@@ -143,6 +143,36 @@
   </si>
   <si>
     <t>4.89 min</t>
+  </si>
+  <si>
+    <t>50000 (unlabeled)</t>
+  </si>
+  <si>
+    <t>2.436 h</t>
+  </si>
+  <si>
+    <t>1.360h</t>
+  </si>
+  <si>
+    <t>44.81 min</t>
+  </si>
+  <si>
+    <t>28.51min</t>
+  </si>
+  <si>
+    <t>26.71min</t>
+  </si>
+  <si>
+    <t>9.24min</t>
+  </si>
+  <si>
+    <t>2.58h</t>
+  </si>
+  <si>
+    <t>2.085h</t>
+  </si>
+  <si>
+    <t>1.682h</t>
   </si>
 </sst>
 </file>
@@ -190,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -202,9 +232,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -490,7 +517,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,14 +728,127 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" s="4"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="5"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>13500</v>
+      </c>
+      <c r="C17" s="3">
+        <v>10000</v>
+      </c>
+      <c r="D17" s="3">
+        <v>7500</v>
+      </c>
+      <c r="E17" s="3">
+        <v>5000</v>
+      </c>
+      <c r="F17" s="3">
+        <v>2500</v>
+      </c>
+      <c r="G17" s="3">
+        <v>500</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3">
+        <v>9.69</v>
+      </c>
+      <c r="C18" s="3">
+        <v>5.25</v>
+      </c>
+      <c r="D18" s="3">
+        <v>6.33</v>
+      </c>
+      <c r="E18" s="3">
+        <v>3.81</v>
+      </c>
+      <c r="F18" s="3">
+        <v>3.08</v>
+      </c>
+      <c r="G18" s="3">
+        <v>2.17</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="3">
+        <v>10.09</v>
+      </c>
+      <c r="C20" s="4">
+        <v>7.16</v>
+      </c>
+      <c r="D20" s="3">
+        <v>6.36</v>
+      </c>
+      <c r="E20" s="3">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="F20" s="3">
+        <v>2.93</v>
+      </c>
+      <c r="G20" s="3">
+        <v>2.37</v>
+      </c>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="3">
+        <v>48.5</v>
+      </c>
+      <c r="F21" s="3">
+        <v>14.94</v>
+      </c>
+      <c r="G21" s="3">
+        <v>6.03</v>
+      </c>
+      <c r="H21" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sobol GP and DNN updated, results obtained for 5000 samples
</commit_message>
<xml_diff>
--- a/results/Lake/ComputationalTime.xlsx
+++ b/results/Lake/ComputationalTime.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20356"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1511ED44-0A8F-4B7A-A99B-9566BC7CF174}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E959EB81-1ACA-40B1-A355-172ACBBE7736}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="6795" windowHeight="7290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="139">
   <si>
     <t xml:space="preserve">DNN_loss_MC_p_Lake.py </t>
   </si>
@@ -173,6 +173,270 @@
   </si>
   <si>
     <t>1.682h</t>
+  </si>
+  <si>
+    <t>Time difference of 7.936687 mins</t>
+  </si>
+  <si>
+    <t>Warning message in write.table(dat, filename, sep = ",", col.names = !file.exists(filename), :</t>
+  </si>
+  <si>
+    <t>"appending column names to file"Warning message in write.table(datT, filenameT, sep = ",", col.names = !file.exists(filenameT), :</t>
+  </si>
+  <si>
+    <t>"appending column names to file"</t>
+  </si>
+  <si>
+    <t>Time difference of 5.361337 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 4.720694 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 3.760925 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 22.23672 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 9.576608 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 9.315822 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 5.372882 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 7.250577 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 6.067961 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 4.482874 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 3.92888 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 28.54099 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 8.670549 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 7.466797 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 5.089095 mins</t>
+  </si>
+  <si>
+    <t>10000 nsim</t>
+  </si>
+  <si>
+    <t>numobs &lt;- c(7500,5000,2500,500)</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
+  <si>
+    <t>3hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GP_MC_p_Lake.py </t>
+  </si>
+  <si>
+    <t>Time difference of 38.07757 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 38.98227 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 45.60727 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 53.94873 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 1.088922 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GP_loss_MC_p_Lake.py </t>
+  </si>
+  <si>
+    <t>Time difference of 39.62221 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 41.5744 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 52.98217 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 1.102614 hours</t>
+  </si>
+  <si>
+    <t>Time difference of 1.380533 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GP_upd_MC_p_Lake.py </t>
+  </si>
+  <si>
+    <t>Time difference of 37.10994 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 37.9674 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 42.3716 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 51.81466 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 1.073198 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GP_upd_loss_MC_p_Lake.py </t>
+  </si>
+  <si>
+    <t>Time difference of 36.70206 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 38.00842 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 41.92811 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 50.99133 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 1.024513 hours</t>
+  </si>
+  <si>
+    <t>Time difference of 2.393318 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 2.23173 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 2.383795 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 2.590194 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 2.800797 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 4.159789 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 4.334317 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 5.117816 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 5.910678 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 6.701035 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 2.447957 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 2.453634 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 2.606229 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 2.93356 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 2.868415 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 4.792869 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 4.916013 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 6.450937 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 7.238759 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 7.059769 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 38.09898 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 40.46431 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 50.10835 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 1.122853 hours</t>
+  </si>
+  <si>
+    <t>Time difference of 1.463256 hours</t>
+  </si>
+  <si>
+    <t>Time difference of 40.78493 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 45.17108 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 1.072812 hours</t>
+  </si>
+  <si>
+    <t>Time difference of 1.510213 hours</t>
+  </si>
+  <si>
+    <t>Time difference of 2.041269 hours</t>
+  </si>
+  <si>
+    <t>Time difference of 36.86042 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 39.32713 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 46.424 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 57.87917 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 1.294667 hours</t>
+  </si>
+  <si>
+    <t>Time difference of 37.0452 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 38.60814 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 46.23448 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 58.17413 mins</t>
+  </si>
+  <si>
+    <t>Time difference of 1.319228 hours</t>
+  </si>
+  <si>
+    <t>5000 and 10 restart</t>
   </si>
 </sst>
 </file>
@@ -514,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H191"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,6 +1114,766 @@
       </c>
       <c r="H21" s="3"/>
     </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>3</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>4</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>